<commit_message>
restore last changes from Douglas
</commit_message>
<xml_diff>
--- a/4 Bring Up/Bring Up Change List REV 1.xlsx
+++ b/4 Bring Up/Bring Up Change List REV 1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="1920" yWindow="0" windowWidth="26020" windowHeight="15260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -282,23 +282,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -306,11 +306,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -319,7 +319,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -327,17 +327,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -347,7 +347,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -355,12 +355,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -369,35 +369,35 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,20 +806,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="29.375" customWidth="1"/>
-    <col min="3" max="3" width="50.125" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="88.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5" customWidth="1"/>
     <col min="5" max="5" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="16.5">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -830,7 +830,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="16.5">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -841,7 +841,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.5">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -852,7 +852,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16.5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -861,7 +861,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16.5">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="48">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -893,7 +893,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
@@ -912,7 +912,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -950,7 +950,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
@@ -969,7 +969,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="15" t="s">
         <v>9</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="15" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="15" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="F13" s="9"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="15" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="18" t="s">
         <v>9</v>
       </c>
@@ -1064,7 +1064,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="15" t="s">
         <v>9</v>
       </c>
@@ -1083,7 +1083,7 @@
       <c r="F16" s="9"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="15" t="s">
         <v>9</v>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="15" t="s">
         <v>9</v>
       </c>
@@ -1121,7 +1121,7 @@
       <c r="F18" s="9"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="15" t="s">
         <v>9</v>
       </c>
@@ -1140,7 +1140,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="20" t="s">
         <v>9</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="25" t="s">
         <v>44</v>
       </c>
@@ -1176,7 +1176,7 @@
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="25" t="s">
         <v>44</v>
       </c>
@@ -1189,7 +1189,7 @@
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="25" t="s">
         <v>44</v>
       </c>
@@ -1202,7 +1202,7 @@
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="25" t="s">
         <v>44</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="25" t="s">
         <v>44</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7">
       <c r="A26" s="25" t="s">
         <v>44</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="25" t="s">
         <v>44</v>
       </c>
@@ -1254,7 +1254,7 @@
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="25" t="s">
         <v>44</v>
       </c>
@@ -1267,7 +1267,7 @@
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="25" t="s">
         <v>44</v>
       </c>
@@ -1280,7 +1280,7 @@
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="25" t="s">
         <v>44</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="25" t="s">
         <v>44</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="25" t="s">
         <v>44</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="25" t="s">
         <v>44</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="25" t="s">
         <v>44</v>
       </c>
@@ -1347,7 +1347,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Revert "restore last changes from Douglas"
This reverts commit fe8e9e2b7e6a1e2b61edefbca5f57cdcf2c6712e.
</commit_message>
<xml_diff>
--- a/4 Bring Up/Bring Up Change List REV 1.xlsx
+++ b/4 Bring Up/Bring Up Change List REV 1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="0" windowWidth="26020" windowHeight="15260" tabRatio="500"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -282,23 +282,23 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -306,11 +306,11 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -319,7 +319,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -327,17 +327,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -347,7 +347,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -355,12 +355,12 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -369,35 +369,35 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -806,20 +806,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="29.33203125" customWidth="1"/>
-    <col min="3" max="3" width="88.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.375" customWidth="1"/>
+    <col min="3" max="3" width="50.125" customWidth="1"/>
     <col min="4" max="4" width="38.5" customWidth="1"/>
     <col min="5" max="5" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5">
+    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -830,7 +830,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="16.5">
+    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -841,7 +841,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="16.5">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -852,7 +852,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -861,7 +861,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5">
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -872,7 +872,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="48">
+    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -893,7 +893,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>9</v>
       </c>
@@ -912,7 +912,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>9</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
@@ -950,7 +950,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
@@ -969,7 +969,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>9</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="F11" s="9"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="F13" s="9"/>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1045,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>9</v>
       </c>
@@ -1064,7 +1064,7 @@
       <c r="F15" s="9"/>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>9</v>
       </c>
@@ -1083,7 +1083,7 @@
       <c r="F16" s="9"/>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>9</v>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="F17" s="9"/>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>9</v>
       </c>
@@ -1121,7 +1121,7 @@
       <c r="F18" s="9"/>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="16" thickBot="1">
+    <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>9</v>
       </c>
@@ -1140,7 +1140,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="16" thickBot="1">
+    <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>9</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>44</v>
       </c>
@@ -1176,7 +1176,7 @@
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>44</v>
       </c>
@@ -1189,7 +1189,7 @@
       <c r="D22" s="27"/>
       <c r="E22" s="27"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>44</v>
       </c>
@@ -1202,7 +1202,7 @@
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>44</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>44</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>44</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>44</v>
       </c>
@@ -1254,7 +1254,7 @@
       <c r="D27" s="27"/>
       <c r="E27" s="27"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>44</v>
       </c>
@@ -1267,7 +1267,7 @@
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>44</v>
       </c>
@@ -1280,7 +1280,7 @@
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>44</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>44</v>
       </c>
@@ -1306,7 +1306,7 @@
       <c r="D31" s="27"/>
       <c r="E31" s="27"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>44</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>44</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>44</v>
       </c>
@@ -1347,7 +1347,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>